<commit_message>
Bank, ATM, Customer, Transaction working
</commit_message>
<xml_diff>
--- a/bankingTransaction/checklist_bank.xlsx
+++ b/bankingTransaction/checklist_bank.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\trainee\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12435" windowHeight="2475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="20">
   <si>
     <t>Bank</t>
   </si>
@@ -78,6 +74,12 @@
   </si>
   <si>
     <t>commits</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>generateReport</t>
   </si>
 </sst>
 </file>
@@ -121,9 +123,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,13 +414,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -470,48 +479,240 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated 21 may 7pm
</commit_message>
<xml_diff>
--- a/bankingTransaction/checklist_bank.xlsx
+++ b/bankingTransaction/checklist_bank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12435" windowHeight="2475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="20">
   <si>
     <t>Bank</t>
   </si>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,10 +486,18 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -504,10 +512,18 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -555,8 +571,12 @@
       <c r="L6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="M6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -595,8 +615,12 @@
       <c r="L7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="M7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -613,8 +637,8 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -631,8 +655,8 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -671,8 +695,12 @@
       <c r="L10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="M10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -711,8 +739,12 @@
       <c r="L11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="M11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>